<commit_message>
changes hopefully this fixes
</commit_message>
<xml_diff>
--- a/Green Line Info_.xlsx
+++ b/Green Line Info_.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\School\1140\1140\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\School\1140\1140_iteration4\1140\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6433B45C-CA55-40EE-8561-9C07DEB8A147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4B131F-9DEC-48BC-972F-271BE62DE00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
+    <workbookView xWindow="492" yWindow="912" windowWidth="17280" windowHeight="8964" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="49">
   <si>
     <t>Section</t>
   </si>
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4104CD2-E043-4597-AF7D-F6AD80AEEABB}">
-  <dimension ref="A1:E223"/>
+  <dimension ref="A1:E224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="E209" sqref="E209"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174:E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3206,41 +3206,44 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B174" s="3">
-        <v>58</v>
-      </c>
-      <c r="C174" s="3">
-        <v>50</v>
-      </c>
-      <c r="D174" s="3">
-        <v>60</v>
-      </c>
-      <c r="E174" s="5" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="B174" s="5">
+        <v>151</v>
+      </c>
+      <c r="C174" s="5">
+        <v>50</v>
+      </c>
+      <c r="D174" s="5">
+        <v>100</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B175" s="4">
-        <v>59</v>
+      <c r="B175" s="3">
+        <v>58</v>
       </c>
       <c r="C175" s="3">
         <v>50</v>
       </c>
       <c r="D175" s="3">
         <v>60</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B176" s="3">
-        <v>60</v>
+      <c r="B176" s="4">
+        <v>59</v>
       </c>
       <c r="C176" s="3">
         <v>50</v>
@@ -3254,17 +3257,28 @@
         <v>12</v>
       </c>
       <c r="B177" s="3">
+        <v>60</v>
+      </c>
+      <c r="C177" s="3">
+        <v>50</v>
+      </c>
+      <c r="D177" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B178" s="3">
         <v>61</v>
       </c>
-      <c r="C177" s="3">
-        <v>50</v>
-      </c>
-      <c r="D177" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D193" s="3"/>
+      <c r="C178" s="3">
+        <v>50</v>
+      </c>
+      <c r="D178" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="194" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D194" s="3"/>
@@ -3284,41 +3298,38 @@
     <row r="199" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D199" s="3"/>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A212" s="3"/>
-      <c r="B212" s="4"/>
-      <c r="C212" s="3"/>
-      <c r="D212" s="3"/>
-      <c r="E212" s="5"/>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D200" s="3"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="3"/>
-      <c r="B213" s="3"/>
+      <c r="B213" s="4"/>
       <c r="C213" s="3"/>
       <c r="D213" s="3"/>
+      <c r="E213" s="5"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
       <c r="D214" s="3"/>
-      <c r="E214" s="5"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="3"/>
-      <c r="B215" s="4"/>
+      <c r="B215" s="3"/>
       <c r="C215" s="3"/>
       <c r="D215" s="3"/>
+      <c r="E215" s="5"/>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="3"/>
-      <c r="B216" s="3"/>
+      <c r="B216" s="4"/>
       <c r="C216" s="3"/>
       <c r="D216" s="3"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="3"/>
-      <c r="B217" s="4"/>
+      <c r="B217" s="3"/>
       <c r="C217" s="3"/>
       <c r="D217" s="3"/>
     </row>
@@ -3330,7 +3341,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="3"/>
-      <c r="B219" s="3"/>
+      <c r="B219" s="4"/>
       <c r="C219" s="3"/>
       <c r="D219" s="3"/>
     </row>
@@ -3342,22 +3353,28 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="3"/>
-      <c r="B221" s="4"/>
+      <c r="B221" s="3"/>
       <c r="C221" s="3"/>
       <c r="D221" s="3"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="3"/>
-      <c r="B222" s="3"/>
+      <c r="B222" s="4"/>
       <c r="C222" s="3"/>
       <c r="D222" s="3"/>
-      <c r="E222" s="5"/>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="3"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
       <c r="D223" s="3"/>
+      <c r="E223" s="5"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A224" s="3"/>
+      <c r="B224" s="3"/>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>